<commit_message>
first time run through
</commit_message>
<xml_diff>
--- a/data/SystemParameter.xlsx
+++ b/data/SystemParameter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YuYX\Desktop\CompetitionSystem\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C357683F-C5F1-4ECF-A626-860E9976EF1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F837EDEC-E407-407E-9ECE-94930B93725F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="24300" windowHeight="14856" tabRatio="790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="24300" windowHeight="14856" tabRatio="790" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="规则" sheetId="4" r:id="rId1"/>
@@ -2852,11 +2852,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AL21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4560,11 +4560,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AB20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S13" sqref="S13"/>
+      <selection pane="bottomRight" activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5164,7 +5164,7 @@
         <v>0</v>
       </c>
       <c r="S7" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7" s="3" t="b">
         <v>0</v>
@@ -5822,7 +5822,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>